<commit_message>
New changes to electric
</commit_message>
<xml_diff>
--- a/decarbonize/Electricity Rate Plan.xlsx
+++ b/decarbonize/Electricity Rate Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pragn\OneDrive\Desktop\CarbonSustain\ai-apps\decarbonize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF1B214-8B9B-45DC-A86C-2522431AD87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF2A422-6B06-4CFD-8661-0DD9BBCE8AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,15 +23,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -20736,8 +20727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7BF5F5-9B64-444F-8807-74F4F2EE40E4}">
   <dimension ref="A1:L409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>